<commit_message>
updates through 1/2/24 17:15 - all RecordMsg methods validated
</commit_message>
<xml_diff>
--- a/Code Plan.xlsx
+++ b/Code Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Python_ErrorHandling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BD42A0-3B84-4FC7-8785-1B9BC6364A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B501BEE-99C9-4182-81B6-A540BDB57623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1073" yWindow="1448" windowWidth="28799" windowHeight="11587" xr2:uid="{BC6A1FF8-FCEF-4310-9430-53F13A45C0E8}"/>
+    <workbookView xWindow="2093" yWindow="2467" windowWidth="28800" windowHeight="11588" xr2:uid="{BC6A1FF8-FCEF-4310-9430-53F13A45C0E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Arguments</t>
   </si>
@@ -66,10 +66,6 @@
   </si>
   <si>
     <t>IsHandle</t>
-  </si>
-  <si>
-    <t>Initialize all attributes
-Import Error Codes</t>
   </si>
   <si>
     <t>Initialize class for error handling</t>
@@ -88,6 +84,30 @@
   <si>
     <t>Boolean function to check fail/pass condition (evals True if fail)
 Set class parameters if fail</t>
+  </si>
+  <si>
+    <t>RecordMsg (procedure)</t>
+  </si>
+  <si>
+    <t>Process an error or warning into a msg string</t>
+  </si>
+  <si>
+    <t>Initialize all attributes
+Import Error Codes to .df_errs from Excel file</t>
+  </si>
+  <si>
+    <t>GetBaseErrCode</t>
+  </si>
+  <si>
+    <t>Look up Base .df_errs code for .Locn</t>
+  </si>
+  <si>
+    <t>SetReportErrCode</t>
+  </si>
+  <si>
+    <t>Set iCodeBase to global variable iErrNotFound if no rows match .Locn in the .df_errs "Locn" column
+Set base_row to the .df_errs rows matching .Locn in the "Locn" column and matching "Base" in the Msg_String column
+if base_row is not empty, set .iCodeBase to the .df_errs "iCode" column value for base_row[0]</t>
   </si>
 </sst>
 </file>
@@ -124,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +162,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -196,7 +222,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -216,6 +242,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
@@ -533,13 +560,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62ADAB2-59CA-4D89-A7D5-36DD0F6BBCE7}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -556,7 +583,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>
@@ -593,48 +620,80 @@
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="35.65" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="70.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="35.65" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D7"/>
@@ -696,12 +755,6 @@
       <c r="F16"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
1/3/24 changes --add preflight.py
</commit_message>
<xml_diff>
--- a/Code Plan.xlsx
+++ b/Code Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Python_ErrorHandling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B501BEE-99C9-4182-81B6-A540BDB57623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD04E54A-8CB1-460E-805A-D9F31FE74378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2093" yWindow="2467" windowWidth="28800" windowHeight="11588" xr2:uid="{BC6A1FF8-FCEF-4310-9430-53F13A45C0E8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Arguments</t>
   </si>
@@ -108,6 +108,23 @@
     <t>Set iCodeBase to global variable iErrNotFound if no rows match .Locn in the .df_errs "Locn" column
 Set base_row to the .df_errs rows matching .Locn in the "Locn" column and matching "Base" in the Msg_String column
 if base_row is not empty, set .iCodeBase to the .df_errs "iCode" column value for base_row[0]</t>
+  </si>
+  <si>
+    <t>If iCodeBase is not iErrNotFound, calculate .iCodeReport as sum of .iCodeBase and .iCodeLocal</t>
+  </si>
+  <si>
+    <t>ReportError</t>
+  </si>
+  <si>
+    <t>If .ErrMsg is not empty string, 
+Raise error with that string as user message
+Append .ErrMsg to .ErrMsgsAccum with added new line character if ErrMsgsAccum contains previous text</t>
+  </si>
+  <si>
+    <t>ResetWarning</t>
+  </si>
+  <si>
+    <t>Re-initialize .iCodeBase, .iCodeReport, .iCodeLocal, .ErrMsg and .ErrParam class attributes to their default values as set in .__init()__</t>
   </si>
 </sst>
 </file>
@@ -560,13 +577,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62ADAB2-59CA-4D89-A7D5-36DD0F6BBCE7}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -661,7 +678,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
@@ -671,41 +688,67 @@
       <c r="C5" s="3"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="35.65" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="24" x14ac:dyDescent="0.45">
+      <c r="A7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" ht="35.65" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D9"/>
@@ -755,6 +798,18 @@
       <c r="F16"/>
       <c r="G16"/>
     </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.45">
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.45">
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
changes through 1/12/24 CheckDataFrame methods added
</commit_message>
<xml_diff>
--- a/Code Plan.xlsx
+++ b/Code Plan.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Python_ErrorHandling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD04E54A-8CB1-460E-805A-D9F31FE74378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281FEC18-9288-485B-9664-F0D2EE0C098E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2093" yWindow="2467" windowWidth="28800" windowHeight="11588" xr2:uid="{BC6A1FF8-FCEF-4310-9430-53F13A45C0E8}"/>
+    <workbookView xWindow="735" yWindow="1110" windowWidth="30150" windowHeight="16515" xr2:uid="{BC6A1FF8-FCEF-4310-9430-53F13A45C0E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$17</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>Arguments</t>
   </si>
@@ -48,9 +51,6 @@
   </si>
   <si>
     <t>Internal Variables</t>
-  </si>
-  <si>
-    <t>Test Assert Statements</t>
   </si>
   <si>
     <t>Function Name</t>
@@ -82,16 +82,6 @@
 Set.ErrParam if specified in is_fail arguments</t>
   </si>
   <si>
-    <t>Boolean function to check fail/pass condition (evals True if fail)
-Set class parameters if fail</t>
-  </si>
-  <si>
-    <t>RecordMsg (procedure)</t>
-  </si>
-  <si>
-    <t>Process an error or warning into a msg string</t>
-  </si>
-  <si>
     <t>Initialize all attributes
 Import Error Codes to .df_errs from Excel file</t>
   </si>
@@ -125,6 +115,109 @@
   </si>
   <si>
     <t>Re-initialize .iCodeBase, .iCodeReport, .iCodeLocal, .ErrMsg and .ErrParam class attributes to their default values as set in .__init()__</t>
+  </si>
+  <si>
+    <t>RecordErr (procedure)</t>
+  </si>
+  <si>
+    <t>Procedure to record/report an error or warning</t>
+  </si>
+  <si>
+    <t>Sets the report error code as the sum of base and local error codes</t>
+  </si>
+  <si>
+    <t>AppendErrMsg</t>
+  </si>
+  <si>
+    <t>Append error message for iCodeReport</t>
+  </si>
+  <si>
+    <t>Reports an error based on the ErrMsg attribute</t>
+  </si>
+  <si>
+    <t>Reset attributes to default values after reporting non-fatal/warning</t>
+  </si>
+  <si>
+    <t>Boolean check condition; return True and  set class params if fail
+Set class parameters if fail</t>
+  </si>
+  <si>
+    <t>CheckExcelFiles</t>
+  </si>
+  <si>
+    <t>lst_files
+lst_shts
+errs</t>
+  </si>
+  <si>
+    <t>Initialize CheckExcelFiles with a list of file paths and a list of sheets for each file
+Set class parameters if fail</t>
+  </si>
+  <si>
+    <t>CheckFilesProcedure</t>
+  </si>
+  <si>
+    <t>Procedure to check specified Excel files and sheets</t>
+  </si>
+  <si>
+    <t>iterate idx over the list index of .lst_files and:
+Call .ExcelFileExists method for idx
+Call .ExcelFileOpens method for idx
+If the file exists and is valid, call .AllSheetsExist() method to check that specified list from .lst_shts exists for list index idx</t>
+  </si>
+  <si>
+    <t>ExcelFileExists</t>
+  </si>
+  <si>
+    <t>ExcelFileOpens</t>
+  </si>
+  <si>
+    <t>AllSheetsExist</t>
+  </si>
+  <si>
+    <t>SheetExists</t>
+  </si>
+  <si>
+    <t>Check if an Excel file exists based on specified list index for list of files to check (iteration over list in calling CheckFilesProcedure)</t>
+  </si>
+  <si>
+    <t>Check if file is a valid Excel file based on ability to open</t>
+  </si>
+  <si>
+    <t>Iteratively check if specified sheets exist in self.wb</t>
+  </si>
+  <si>
+    <t>Check if specified sheet exists in self.wb</t>
+  </si>
+  <si>
+    <t>CheckDataFrame</t>
+  </si>
+  <si>
+    <t>ColNonBlank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check </t>
+  </si>
+  <si>
+    <t>Initialize CheckDataFrame with df  and errs ErrorHandle instance as attributes</t>
+  </si>
+  <si>
+    <t>Test Instructions</t>
+  </si>
+  <si>
+    <t>test that the class was instanced properly</t>
+  </si>
+  <si>
+    <t>df; errs</t>
+  </si>
+  <si>
+    <t>Initialize all attributes; Import Error Codes to .df_errs from Excel file</t>
+  </si>
+  <si>
+    <t>Check that a DataFrame column contains at least one non-blank value</t>
+  </si>
+  <si>
+    <t>ContainsRequiredCols</t>
   </si>
 </sst>
 </file>
@@ -239,7 +332,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -260,6 +353,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
@@ -576,14 +672,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62ADAB2-59CA-4D89-A7D5-36DD0F6BBCE7}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H18"/>
+  <sheetPr codeName="Sheet1" filterMode="1"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -598,12 +694,12 @@
     <col min="8" max="8" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -618,199 +714,319 @@
         <v>2</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="24" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="70.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="70.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="24" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="24" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" ht="47.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="35.65" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
+    <row r="8" spans="1:9" ht="24" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.45">
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-    </row>
+    <row r="9" spans="1:9" ht="35.65" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" ht="35.65" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" ht="58.9" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" ht="24" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" ht="24" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:8" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A17" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
+  <autoFilter ref="A1:I17" xr:uid="{B62ADAB2-59CA-4D89-A7D5-36DD0F6BBCE7}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="CheckDataFrame"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>